<commit_message>
my analysis of alternates work
</commit_message>
<xml_diff>
--- a/CH-066 Merged cells.xlsx
+++ b/CH-066 Merged cells.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333A18CF-F70D-4705-9A99-F1D43306C18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6335B786-814A-4EFD-BA2C-7FFDDECD73C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26940" yWindow="195" windowWidth="23115" windowHeight="12735" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -1012,6 +1012,35 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{15B6BE95-CDD2-4371-BF5A-63F102A12747}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{74312796-FE0F-45F6-9824-E23BA03E0A65}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R26"/>
@@ -2056,7 +2085,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2783,10 +2812,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E871E53-38B8-4068-BFB3-8EFA6F89D12B}">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3269,222 +3298,67 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="4" t="str" cm="1">
-        <f t="array" ref="B22:E36">_xlfn.LET(_xlpm.d,B4:B8,_xlpm.u,_xlfn.UNIQUE(C3:G3,1),_xlfn.HSTACK(_xlfn.TOCOL(_xlpm.d&amp;T(_xlpm.u),,1),_xlfn.TOCOL(_xlpm.u+N(+_xlpm.d),,1),_xlfn.TOCOL(_xlfn.EXPAND(C4:D8,,3,""),,1),_xlfn.TOCOL(E4:G8,,1)))</f>
-        <v>Sales</v>
+      <c r="B22" s="4" cm="1">
+        <f t="array" ref="B22:D26">_xlfn.LET(_xlpm.d, B4:B8, _xlpm.u, _xlfn.UNIQUE(C3:G3, 1), _xlpm.z, _xlfn.HSTACK(_xlfn.TOCOL(_xlpm.d &amp; T(_xlpm.u), , 1), _xlfn.TOCOL(_xlpm.u + N(+_xlpm.d), , 1), _xlfn.TOCOL(_xlfn.EXPAND(C4:D8, , 3, ""), , 1), _xlfn.TOCOL(E4:G8, , 1)), _xlfn.EXPAND(C4:D8, , 3, ""))</f>
+        <v>89</v>
       </c>
       <c r="C22" s="4">
-        <v>2022</v>
-      </c>
-      <c r="D22" s="4">
-        <v>89</v>
-      </c>
-      <c r="E22" s="4">
-        <v>53</v>
+        <v>83</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <v/>
       </c>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="4" t="str">
-        <v>Marketing</v>
+      <c r="B23" s="4">
+        <v>67</v>
       </c>
       <c r="C23" s="4">
-        <v>2022</v>
-      </c>
-      <c r="D23" s="4">
-        <v>67</v>
-      </c>
-      <c r="E23" s="4">
-        <v>80</v>
+        <v>70</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <v/>
       </c>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="4" t="str">
-        <v>IT</v>
+      <c r="B24" s="4">
+        <v>29</v>
       </c>
       <c r="C24" s="4">
-        <v>2022</v>
-      </c>
-      <c r="D24" s="4">
-        <v>29</v>
-      </c>
-      <c r="E24" s="4">
-        <v>67</v>
+        <v>96</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <v/>
       </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="str">
-        <v>Production</v>
+      <c r="B25" s="4">
+        <v>18</v>
       </c>
       <c r="C25" s="4">
-        <v>2022</v>
-      </c>
-      <c r="D25" s="4">
-        <v>18</v>
-      </c>
-      <c r="E25" s="4">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="D25" s="4" t="str">
+        <v/>
       </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="str">
-        <v>R&amp;D</v>
+      <c r="B26" s="4">
+        <v>25</v>
       </c>
       <c r="C26" s="4">
-        <v>2022</v>
-      </c>
-      <c r="D26" s="4">
-        <v>25</v>
-      </c>
-      <c r="E26" s="4">
-        <v>90</v>
+        <v>40</v>
+      </c>
+      <c r="D26" s="4" t="str">
+        <v/>
       </c>
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="str">
-        <v>Sales</v>
-      </c>
-      <c r="C27" s="4">
-        <v>2023</v>
-      </c>
-      <c r="D27" s="4">
-        <v>83</v>
-      </c>
-      <c r="E27" s="4">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="str">
-        <v>Marketing</v>
-      </c>
-      <c r="C28" s="4">
-        <v>2023</v>
-      </c>
-      <c r="D28" s="4">
-        <v>70</v>
-      </c>
-      <c r="E28" s="4">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="str">
-        <v>IT</v>
-      </c>
-      <c r="C29" s="4">
-        <v>2023</v>
-      </c>
-      <c r="D29" s="4">
-        <v>96</v>
-      </c>
-      <c r="E29" s="4">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="str">
-        <v>Production</v>
-      </c>
-      <c r="C30" s="4">
-        <v>2023</v>
-      </c>
-      <c r="D30" s="4">
-        <v>11</v>
-      </c>
-      <c r="E30" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="str">
-        <v>R&amp;D</v>
-      </c>
-      <c r="C31" s="4">
-        <v>2023</v>
-      </c>
-      <c r="D31" s="4">
-        <v>40</v>
-      </c>
-      <c r="E31" s="4">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="str">
-        <v>Sales</v>
-      </c>
-      <c r="C32" s="4">
-        <v>2024</v>
-      </c>
-      <c r="D32" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E32" s="4">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="str">
-        <v>Marketing</v>
-      </c>
-      <c r="C33" s="4">
-        <v>2024</v>
-      </c>
-      <c r="D33" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E33" s="4">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="str">
-        <v>IT</v>
-      </c>
-      <c r="C34" s="4">
-        <v>2024</v>
-      </c>
-      <c r="D34" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E34" s="4">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="str">
-        <v>Production</v>
-      </c>
-      <c r="C35" s="4">
-        <v>2024</v>
-      </c>
-      <c r="D35" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E35" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="str">
-        <v>R&amp;D</v>
-      </c>
-      <c r="C36" s="4">
-        <v>2024</v>
-      </c>
-      <c r="D36" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E36" s="4">
-        <v>43</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3497,4 +3371,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAE0ARABZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74312796-FE0F-45F6-9824-E23BA03E0A65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Worked through how the T and N functions were used to unravel the array
</commit_message>
<xml_diff>
--- a/CH-066 Merged cells.xlsx
+++ b/CH-066 Merged cells.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D07FCD4-61DB-4F66-9C94-F86B9755CB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F47DE1-CED0-4316-8B08-1F5F0FFD372D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46545" yWindow="645" windowWidth="43200" windowHeight="23385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32310" yWindow="1770" windowWidth="28815" windowHeight="15915" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="14">
   <si>
     <t>Question</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Scratchwork</t>
+  </si>
+  <si>
+    <t>This makes a index-counting argument. This would be the first thing I would normally try.</t>
+  </si>
+  <si>
+    <t>Now he uses a similar technique to create an array of numbers</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -504,6 +510,15 @@
     <xf numFmtId="3" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -522,14 +537,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -810,6 +819,88 @@
             </a:rPr>
             <a:t>Convert the Question table with the merge headers into the result table.</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C689C11-C8BF-296F-8DA5-F97DA4569B99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5029200" y="3838575"/>
+          <a:ext cx="3105150" cy="1085850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> was an unusual use of the T() function to turn an array of numbers into blanks. Very clever.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1110,34 +1201,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="I1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="I1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
     </row>
     <row r="2" spans="1:18" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="35"/>
       <c r="I2" s="21" t="s">
         <v>2</v>
       </c>
@@ -1152,7 +1243,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="12">
         <v>2022</v>
       </c>
@@ -1618,7 +1709,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1635,34 +1726,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="I1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="I1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
     </row>
     <row r="2" spans="1:18" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="35"/>
       <c r="I2" s="21" t="s">
         <v>2</v>
       </c>
@@ -1677,7 +1768,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="12">
         <v>2022</v>
       </c>
@@ -2111,6 +2202,9 @@
         <v>Budget</v>
       </c>
       <c r="H21" s="1"/>
+      <c r="I21" s="40" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
@@ -2348,10 +2442,735 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" style="4" customWidth="1"/>
+    <col min="3" max="6" width="6.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="8" width="4" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="6.09765625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="7.19921875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="7.19921875" customWidth="1"/>
+    <col min="17" max="17" width="9.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="I1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+    </row>
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="34"/>
+      <c r="G2" s="35"/>
+      <c r="I2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="37"/>
+      <c r="C3" s="12">
+        <v>2022</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2023</v>
+      </c>
+      <c r="E3" s="12">
+        <v>2022</v>
+      </c>
+      <c r="F3" s="12">
+        <v>2023</v>
+      </c>
+      <c r="G3" s="19">
+        <v>2024</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="25">
+        <v>2022</v>
+      </c>
+      <c r="K3" s="26">
+        <v>89</v>
+      </c>
+      <c r="L3" s="27">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="13">
+        <v>89</v>
+      </c>
+      <c r="D4" s="13">
+        <v>83</v>
+      </c>
+      <c r="E4" s="14">
+        <v>53</v>
+      </c>
+      <c r="F4" s="14">
+        <v>54</v>
+      </c>
+      <c r="G4" s="15">
+        <v>75</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="20">
+        <v>2022</v>
+      </c>
+      <c r="K4" s="13">
+        <v>67</v>
+      </c>
+      <c r="L4" s="28">
+        <v>80</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="8"/>
+    </row>
+    <row r="5" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="13">
+        <v>67</v>
+      </c>
+      <c r="D5" s="13">
+        <v>70</v>
+      </c>
+      <c r="E5" s="14">
+        <v>80</v>
+      </c>
+      <c r="F5" s="14">
+        <v>62</v>
+      </c>
+      <c r="G5" s="15">
+        <v>42</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="20">
+        <v>2022</v>
+      </c>
+      <c r="K5" s="13">
+        <v>29</v>
+      </c>
+      <c r="L5" s="28">
+        <v>67</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="8"/>
+    </row>
+    <row r="6" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="13">
+        <v>29</v>
+      </c>
+      <c r="D6" s="13">
+        <v>96</v>
+      </c>
+      <c r="E6" s="14">
+        <v>67</v>
+      </c>
+      <c r="F6" s="14">
+        <v>18</v>
+      </c>
+      <c r="G6" s="15">
+        <v>77</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="20">
+        <v>2022</v>
+      </c>
+      <c r="K6" s="13">
+        <v>18</v>
+      </c>
+      <c r="L6" s="28">
+        <v>20</v>
+      </c>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="8"/>
+    </row>
+    <row r="7" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="13">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13">
+        <v>11</v>
+      </c>
+      <c r="E7" s="14">
+        <v>20</v>
+      </c>
+      <c r="F7" s="14">
+        <v>55</v>
+      </c>
+      <c r="G7" s="15">
+        <v>35</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="29">
+        <v>2022</v>
+      </c>
+      <c r="K7" s="16">
+        <v>25</v>
+      </c>
+      <c r="L7" s="30">
+        <v>90</v>
+      </c>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="8"/>
+    </row>
+    <row r="8" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="16">
+        <v>25</v>
+      </c>
+      <c r="D8" s="16">
+        <v>40</v>
+      </c>
+      <c r="E8" s="17">
+        <v>90</v>
+      </c>
+      <c r="F8" s="17">
+        <v>46</v>
+      </c>
+      <c r="G8" s="18">
+        <v>43</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="25">
+        <v>2023</v>
+      </c>
+      <c r="K8" s="26">
+        <v>83</v>
+      </c>
+      <c r="L8" s="27">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="20">
+        <v>2023</v>
+      </c>
+      <c r="K9" s="13">
+        <v>70</v>
+      </c>
+      <c r="L9" s="28">
+        <v>62</v>
+      </c>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+    </row>
+    <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="20">
+        <v>2023</v>
+      </c>
+      <c r="K10" s="13">
+        <v>96</v>
+      </c>
+      <c r="L10" s="28">
+        <v>18</v>
+      </c>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+    </row>
+    <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="20">
+        <v>2023</v>
+      </c>
+      <c r="K11" s="13">
+        <v>11</v>
+      </c>
+      <c r="L11" s="28">
+        <v>55</v>
+      </c>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+    </row>
+    <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="29">
+        <v>2023</v>
+      </c>
+      <c r="K12" s="16">
+        <v>40</v>
+      </c>
+      <c r="L12" s="30">
+        <v>46</v>
+      </c>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+    </row>
+    <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="25">
+        <v>2024</v>
+      </c>
+      <c r="K13" s="26"/>
+      <c r="L13" s="27">
+        <v>75</v>
+      </c>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H14" s="9"/>
+      <c r="I14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="20">
+        <v>2024</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="28">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H15" s="9"/>
+      <c r="I15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="20">
+        <v>2024</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="28">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="20">
+        <v>2024</v>
+      </c>
+      <c r="K16" s="13"/>
+      <c r="L16" s="28">
+        <v>35</v>
+      </c>
+      <c r="Q16" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B22)</f>
+        <v>=LET(d, B4:B8, u, UNIQUE(C3:G3, 1), z, HSTACK(TOCOL(d &amp; T(u), , 1), TOCOL(u + N(+d), , 1), TOCOL(EXPAND(C4:D8, , 3, ""), , 1), TOCOL(E4:G8, , 1)), EXPAND(C4:D8, , 3, ""))</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="29">
+        <v>2024</v>
+      </c>
+      <c r="K17" s="16"/>
+      <c r="L17" s="30">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="H19" s="9"/>
+      <c r="Q19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="40" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(I22)</f>
+        <v>=TOCOL(B4:B8&amp;T(UNIQUE(C3:G3,1)),,1)</v>
+      </c>
+      <c r="Q20" s="40" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(Q22)</f>
+        <v>=TOCOL(UNIQUE(C3:G3,1)+N(+B4:B8),,1)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="4" cm="1">
+        <f t="array" ref="B22:D26">_xlfn.LET(_xlpm.d, B4:B8, _xlpm.u, _xlfn.UNIQUE(C3:G3, 1), _xlpm.z, _xlfn.HSTACK(_xlfn.TOCOL(_xlpm.d &amp; T(_xlpm.u), , 1), _xlfn.TOCOL(_xlpm.u + N(+_xlpm.d), , 1), _xlfn.TOCOL(_xlfn.EXPAND(C4:D8, , 3, ""), , 1), _xlfn.TOCOL(E4:G8, , 1)), _xlfn.EXPAND(C4:D8, , 3, ""))</f>
+        <v>89</v>
+      </c>
+      <c r="C22" s="4">
+        <v>83</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <v/>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="40" t="str" cm="1">
+        <f t="array" ref="I22:I36">_xlfn.TOCOL(B4:B8&amp;T(_xlfn.UNIQUE(C3:G3,1)),,1)</f>
+        <v>Sales</v>
+      </c>
+      <c r="Q22" cm="1">
+        <f t="array" ref="Q22:Q36">_xlfn.TOCOL(_xlfn.UNIQUE(C3:G3,1)+N(+B4:B8),,1)</f>
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="4">
+        <v>67</v>
+      </c>
+      <c r="C23" s="4">
+        <v>70</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <v/>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="40" t="str">
+        <v>Marketing</v>
+      </c>
+      <c r="Q23">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="4">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4">
+        <v>96</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <v/>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="40" t="str">
+        <v>IT</v>
+      </c>
+      <c r="Q24">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="4">
+        <v>18</v>
+      </c>
+      <c r="C25" s="4">
+        <v>11</v>
+      </c>
+      <c r="D25" s="4" t="str">
+        <v/>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="40" t="str">
+        <v>Production</v>
+      </c>
+      <c r="Q25">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B26" s="4">
+        <v>25</v>
+      </c>
+      <c r="C26" s="4">
+        <v>40</v>
+      </c>
+      <c r="D26" s="4" t="str">
+        <v/>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="40" t="str">
+        <v>R&amp;D</v>
+      </c>
+      <c r="Q26">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I27" s="40" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="Q27">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I28" s="40" t="str">
+        <v>Marketing</v>
+      </c>
+      <c r="Q28">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I29" s="40" t="str">
+        <v>IT</v>
+      </c>
+      <c r="Q29">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I30" s="40" t="str">
+        <v>Production</v>
+      </c>
+      <c r="Q30">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I31" s="40" t="str">
+        <v>R&amp;D</v>
+      </c>
+      <c r="Q31">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I32" s="40" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="Q32">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="33" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I33" s="40" t="str">
+        <v>Marketing</v>
+      </c>
+      <c r="Q33">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="34" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I34" s="40" t="str">
+        <v>IT</v>
+      </c>
+      <c r="Q34">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="35" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I35" s="40" t="str">
+        <v>Production</v>
+      </c>
+      <c r="Q35">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="36" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I36" s="40" t="str">
+        <v>R&amp;D</v>
+      </c>
+      <c r="Q36">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="37" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I37" s="40"/>
+    </row>
+    <row r="38" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I38" s="40"/>
+    </row>
+    <row r="39" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I39" s="40"/>
+    </row>
+    <row r="40" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I40" s="40"/>
+    </row>
+    <row r="41" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I41" s="40"/>
+    </row>
+    <row r="42" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I42" s="40"/>
+    </row>
+    <row r="43" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I43" s="40"/>
+    </row>
+    <row r="44" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I44" s="40"/>
+    </row>
+    <row r="45" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I45" s="40"/>
+    </row>
+    <row r="46" spans="9:17" x14ac:dyDescent="0.3">
+      <c r="I46" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6264A6B7-19D7-46FD-981B-E23AC127A496}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:R50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2368,34 +3187,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="I1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="I1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
     </row>
     <row r="2" spans="1:18" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="35"/>
       <c r="I2" s="21" t="s">
         <v>2</v>
       </c>
@@ -2410,7 +3229,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="12">
         <v>2022</v>
       </c>
@@ -2438,6 +3257,10 @@
       </c>
       <c r="L3" s="27">
         <v>53</v>
+      </c>
+      <c r="N3" s="2" t="b">
+        <f>ISNUMBER(J3)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
@@ -2555,7 +3378,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
-      <c r="R6" s="8"/>
+      <c r="R6" s="33"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
@@ -2830,577 +3653,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="4" cm="1">
-        <f t="array" ref="B22:D26">_xlfn.LET(_xlpm.d, B4:B8, _xlpm.u, _xlfn.UNIQUE(C3:G3, 1), _xlpm.z, _xlfn.HSTACK(_xlfn.TOCOL(_xlpm.d &amp; T(_xlpm.u), , 1), _xlfn.TOCOL(_xlpm.u + N(+_xlpm.d), , 1), _xlfn.TOCOL(_xlfn.EXPAND(C4:D8, , 3, ""), , 1), _xlfn.TOCOL(E4:G8, , 1)), _xlfn.EXPAND(C4:D8, , 3, ""))</f>
-        <v>89</v>
-      </c>
-      <c r="C22" s="4">
-        <v>83</v>
-      </c>
-      <c r="D22" s="4" t="str">
-        <v/>
-      </c>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="4">
-        <v>67</v>
-      </c>
-      <c r="C23" s="4">
-        <v>70</v>
-      </c>
-      <c r="D23" s="4" t="str">
-        <v/>
-      </c>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="4">
-        <v>29</v>
-      </c>
-      <c r="C24" s="4">
-        <v>96</v>
-      </c>
-      <c r="D24" s="4" t="str">
-        <v/>
-      </c>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="4">
-        <v>18</v>
-      </c>
-      <c r="C25" s="4">
-        <v>11</v>
-      </c>
-      <c r="D25" s="4" t="str">
-        <v/>
-      </c>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="4">
-        <v>25</v>
-      </c>
-      <c r="C26" s="4">
-        <v>40</v>
-      </c>
-      <c r="D26" s="4" t="str">
-        <v/>
-      </c>
-      <c r="H26" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:G2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6264A6B7-19D7-46FD-981B-E23AC127A496}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:R50"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.09765625" customWidth="1"/>
-    <col min="2" max="2" width="10.59765625" style="4" customWidth="1"/>
-    <col min="3" max="6" width="6.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.5" customWidth="1"/>
-    <col min="8" max="8" width="4" customWidth="1"/>
-    <col min="9" max="9" width="9.59765625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="6.09765625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="7.19921875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="7.19921875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="I1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-    </row>
-    <row r="2" spans="1:18" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-      <c r="I2" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
-      <c r="C3" s="12">
-        <v>2022</v>
-      </c>
-      <c r="D3" s="12">
-        <v>2023</v>
-      </c>
-      <c r="E3" s="12">
-        <v>2022</v>
-      </c>
-      <c r="F3" s="12">
-        <v>2023</v>
-      </c>
-      <c r="G3" s="19">
-        <v>2024</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="25">
-        <v>2022</v>
-      </c>
-      <c r="K3" s="26">
-        <v>89</v>
-      </c>
-      <c r="L3" s="27">
-        <v>53</v>
-      </c>
-      <c r="N3" s="2" t="b">
-        <f>ISNUMBER(J3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="13">
-        <v>89</v>
-      </c>
-      <c r="D4" s="13">
-        <v>83</v>
-      </c>
-      <c r="E4" s="14">
-        <v>53</v>
-      </c>
-      <c r="F4" s="14">
-        <v>54</v>
-      </c>
-      <c r="G4" s="15">
-        <v>75</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="20">
-        <v>2022</v>
-      </c>
-      <c r="K4" s="13">
-        <v>67</v>
-      </c>
-      <c r="L4" s="28">
-        <v>80</v>
-      </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="8"/>
-    </row>
-    <row r="5" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="13">
-        <v>67</v>
-      </c>
-      <c r="D5" s="13">
-        <v>70</v>
-      </c>
-      <c r="E5" s="14">
-        <v>80</v>
-      </c>
-      <c r="F5" s="14">
-        <v>62</v>
-      </c>
-      <c r="G5" s="15">
-        <v>42</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="20">
-        <v>2022</v>
-      </c>
-      <c r="K5" s="13">
-        <v>29</v>
-      </c>
-      <c r="L5" s="28">
-        <v>67</v>
-      </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="8"/>
-    </row>
-    <row r="6" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="13">
-        <v>29</v>
-      </c>
-      <c r="D6" s="13">
-        <v>96</v>
-      </c>
-      <c r="E6" s="14">
-        <v>67</v>
-      </c>
-      <c r="F6" s="14">
-        <v>18</v>
-      </c>
-      <c r="G6" s="15">
-        <v>77</v>
-      </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="20">
-        <v>2022</v>
-      </c>
-      <c r="K6" s="13">
-        <v>18</v>
-      </c>
-      <c r="L6" s="28">
-        <v>20</v>
-      </c>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="39"/>
-    </row>
-    <row r="7" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="13">
-        <v>18</v>
-      </c>
-      <c r="D7" s="13">
-        <v>11</v>
-      </c>
-      <c r="E7" s="14">
-        <v>20</v>
-      </c>
-      <c r="F7" s="14">
-        <v>55</v>
-      </c>
-      <c r="G7" s="15">
-        <v>35</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="29">
-        <v>2022</v>
-      </c>
-      <c r="K7" s="16">
-        <v>25</v>
-      </c>
-      <c r="L7" s="30">
-        <v>90</v>
-      </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="8"/>
-    </row>
-    <row r="8" spans="1:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="16">
-        <v>25</v>
-      </c>
-      <c r="D8" s="16">
-        <v>40</v>
-      </c>
-      <c r="E8" s="17">
-        <v>90</v>
-      </c>
-      <c r="F8" s="17">
-        <v>46</v>
-      </c>
-      <c r="G8" s="18">
-        <v>43</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="25">
-        <v>2023</v>
-      </c>
-      <c r="K8" s="26">
-        <v>83</v>
-      </c>
-      <c r="L8" s="27">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="20">
-        <v>2023</v>
-      </c>
-      <c r="K9" s="13">
-        <v>70</v>
-      </c>
-      <c r="L9" s="28">
-        <v>62</v>
-      </c>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-    </row>
-    <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="20">
-        <v>2023</v>
-      </c>
-      <c r="K10" s="13">
-        <v>96</v>
-      </c>
-      <c r="L10" s="28">
-        <v>18</v>
-      </c>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-    </row>
-    <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J11" s="20">
-        <v>2023</v>
-      </c>
-      <c r="K11" s="13">
-        <v>11</v>
-      </c>
-      <c r="L11" s="28">
-        <v>55</v>
-      </c>
-      <c r="M11"/>
-      <c r="N11"/>
-      <c r="O11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
-      <c r="R11"/>
-    </row>
-    <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="29">
-        <v>2023</v>
-      </c>
-      <c r="K12" s="16">
-        <v>40</v>
-      </c>
-      <c r="L12" s="30">
-        <v>46</v>
-      </c>
-      <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-      <c r="R12"/>
-    </row>
-    <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="J13" s="25">
-        <v>2024</v>
-      </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27">
-        <v>75</v>
-      </c>
-      <c r="M13"/>
-      <c r="N13"/>
-      <c r="O13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
-      <c r="R13"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H14" s="9"/>
-      <c r="I14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="20">
-        <v>2024</v>
-      </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="28">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H15" s="9"/>
-      <c r="I15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J15" s="20">
-        <v>2024</v>
-      </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="28">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J16" s="20">
-        <v>2024</v>
-      </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="28">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="29">
-        <v>2024</v>
-      </c>
-      <c r="K17" s="16"/>
-      <c r="L17" s="30">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="31" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="1"/>
@@ -3841,7 +4094,7 @@
       </c>
     </row>
     <row r="50" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I50" s="38"/>
+      <c r="I50" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>